<commit_message>
[ng-anhhtuann] Viewable prediction vs data dictionary
</commit_message>
<xml_diff>
--- a/elderly-stroke/files-and-variables.xlsx
+++ b/elderly-stroke/files-and-variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macad/Documents/University/Thesis/ECG Processing/elderly-stroke/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7433908-A1DA-E54A-8201-F9ED3C552BBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466DA842-181F-FA4C-8DC0-DAA41A7CD064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="520" windowWidth="38400" windowHeight="21100" tabRatio="993" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Protocol and timeline" sheetId="1" r:id="rId1"/>
@@ -3562,7 +3562,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3591,6 +3591,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -3703,27 +3715,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="18" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3824,7 +3817,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3836,6 +3828,32 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="7"/>
     </xf>
+    <xf numFmtId="18" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -4269,8 +4287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView topLeftCell="A74" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E78" sqref="E78:E95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4289,173 +4307,173 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="10"/>
+      <c r="A5" s="51"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" ht="51.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="12" t="s">
+      <c r="B8" s="6"/>
+      <c r="C8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="12" t="s">
+      <c r="E8" s="6"/>
+      <c r="F8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="13"/>
+      <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="12" t="s">
+      <c r="A9" s="7"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="13"/>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" ht="35.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="12" t="s">
+      <c r="A10" s="7"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="13"/>
+      <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7" ht="10.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="15"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="17" t="s">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="16"/>
+      <c r="G11" s="9"/>
     </row>
     <row r="13" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
     </row>
     <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
@@ -4468,528 +4486,545 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="23" t="s">
+      <c r="D19" s="16" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="5">
+      <c r="B20" s="50">
         <v>0.29166666666666702</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="6"/>
+      <c r="D20" s="51"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="51"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="24">
+      <c r="B22" s="17">
         <v>0.3125</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="17"/>
+      <c r="D22" s="10"/>
     </row>
     <row r="23" spans="1:5" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="25">
+      <c r="B23" s="18">
         <v>0.32638888888888901</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="5" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="B25" s="27"/>
-      <c r="C25" s="17" t="s">
+      <c r="B25" s="20"/>
+      <c r="C25" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="17"/>
+      <c r="D25" s="10"/>
     </row>
     <row r="26" spans="1:5" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="4">
+      <c r="B26" s="54">
         <v>0.33333333333333298</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="51" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="B27" s="4"/>
-      <c r="C27" s="12" t="s">
+      <c r="B27" s="54"/>
+      <c r="C27" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="6"/>
+      <c r="D27" s="51"/>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="B28" s="4"/>
-      <c r="C28" s="12" t="s">
+      <c r="B28" s="54"/>
+      <c r="C28" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D28" s="6"/>
+      <c r="D28" s="51"/>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="B29" s="4"/>
-      <c r="C29" s="12" t="s">
+      <c r="B29" s="54"/>
+      <c r="C29" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="6"/>
+      <c r="D29" s="51"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B30" s="4"/>
-      <c r="C30" s="12" t="s">
+      <c r="B30" s="54"/>
+      <c r="C30" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D30" s="6"/>
+      <c r="D30" s="51"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B31" s="4"/>
-      <c r="C31" s="17" t="s">
+      <c r="B31" s="54"/>
+      <c r="C31" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D31" s="6"/>
+      <c r="D31" s="51"/>
     </row>
     <row r="32" spans="1:5" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="4">
+      <c r="B32" s="54">
         <v>0.35416666666666702</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D32" s="12" t="s">
+      <c r="D32" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E32" s="28"/>
+      <c r="E32" s="21"/>
     </row>
     <row r="33" spans="2:4" ht="55.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="4"/>
-      <c r="C33" s="12" t="s">
+      <c r="B33" s="54"/>
+      <c r="C33" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D33" s="12"/>
+      <c r="D33" s="5"/>
     </row>
     <row r="34" spans="2:4" ht="55.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="4"/>
-      <c r="C34" s="12" t="s">
+      <c r="B34" s="54"/>
+      <c r="C34" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="5" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="B35" s="4"/>
-      <c r="C35" s="12" t="s">
+      <c r="B35" s="54"/>
+      <c r="C35" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D35" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B36" s="4"/>
-      <c r="C36" s="29" t="s">
+      <c r="B36" s="54"/>
+      <c r="C36" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="D36" s="13"/>
+      <c r="D36" s="6"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B37" s="4"/>
-      <c r="C37" s="29" t="s">
+      <c r="B37" s="54"/>
+      <c r="C37" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="D37" s="13"/>
+      <c r="D37" s="6"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B38" s="4"/>
-      <c r="C38" s="30" t="s">
+      <c r="B38" s="54"/>
+      <c r="C38" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D38" s="16"/>
+      <c r="D38" s="9"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B39" s="31">
+      <c r="B39" s="24">
         <v>0.41666666666666702</v>
       </c>
-      <c r="C39" s="17" t="s">
+      <c r="C39" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D39" s="17" t="s">
+      <c r="D39" s="10" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="31">
+      <c r="B40" s="24">
         <v>0.45833333333333298</v>
       </c>
-      <c r="C40" s="17" t="s">
+      <c r="C40" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="D40" s="17" t="s">
+      <c r="D40" s="10" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="3">
+      <c r="B41" s="55">
         <v>0.47916666666666702</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="C41" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D41" s="12" t="s">
+      <c r="D41" s="5" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="3"/>
-      <c r="C42" s="12" t="s">
+      <c r="B42" s="55"/>
+      <c r="C42" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D42" s="12" t="s">
+      <c r="D42" s="5" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="B43" s="3"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="12" t="s">
+      <c r="B43" s="55"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="5" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="11"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="6" t="s">
+      <c r="B44" s="4"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="51" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B45" s="32">
+      <c r="B45" s="25">
         <v>0.5</v>
       </c>
-      <c r="C45" s="17" t="s">
+      <c r="C45" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="D45" s="6"/>
+      <c r="D45" s="51"/>
     </row>
     <row r="46" spans="2:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="2">
+      <c r="B46" s="53">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C46" s="12" t="s">
+      <c r="C46" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D46" s="6" t="s">
+      <c r="D46" s="51" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="48.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="2"/>
-      <c r="C47" s="17" t="s">
+      <c r="B47" s="53"/>
+      <c r="C47" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D47" s="6"/>
+      <c r="D47" s="51"/>
     </row>
     <row r="48" spans="2:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="C48" s="12" t="s">
+      <c r="C48" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="D48" s="51" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B49" s="6"/>
-      <c r="C49" s="12" t="s">
+      <c r="B49" s="51"/>
+      <c r="C49" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D49" s="6"/>
+      <c r="D49" s="51"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B50" s="6"/>
-      <c r="C50" s="12" t="s">
+      <c r="B50" s="51"/>
+      <c r="C50" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D50" s="6"/>
+      <c r="D50" s="51"/>
     </row>
     <row r="51" spans="2:4" ht="45" x14ac:dyDescent="0.2">
-      <c r="B51" s="6"/>
-      <c r="C51" s="17" t="s">
+      <c r="B51" s="51"/>
+      <c r="C51" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="D51" s="6"/>
+      <c r="D51" s="51"/>
     </row>
     <row r="52" spans="2:4" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="33"/>
-      <c r="C52" s="17" t="s">
+      <c r="B52" s="26"/>
+      <c r="C52" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D52" s="17" t="s">
+      <c r="D52" s="10" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="53" spans="2:4" ht="41.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="2">
+      <c r="B53" s="53">
         <v>0.66666666666666696</v>
       </c>
-      <c r="C53" s="12" t="s">
+      <c r="C53" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D53" s="12" t="s">
+      <c r="D53" s="5" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="54" spans="2:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="2"/>
-      <c r="C54" s="12" t="s">
+      <c r="B54" s="53"/>
+      <c r="C54" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D54" s="12" t="s">
+      <c r="D54" s="5" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="55" spans="2:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="B55" s="2"/>
-      <c r="C55" s="17" t="s">
+      <c r="B55" s="53"/>
+      <c r="C55" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="D55" s="16"/>
+      <c r="D55" s="9"/>
     </row>
     <row r="56" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="31">
+      <c r="B56" s="24">
         <v>0.75</v>
       </c>
-      <c r="C56" s="17" t="s">
+      <c r="C56" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="D56" s="17" t="s">
+      <c r="D56" s="10" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="57" spans="2:4" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="2">
+      <c r="B57" s="53">
         <v>0.79166666666666696</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="C57" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="D57" s="6" t="s">
+      <c r="D57" s="51" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B58" s="2"/>
-      <c r="C58" s="6"/>
-      <c r="D58" s="6"/>
+      <c r="B58" s="53"/>
+      <c r="C58" s="51"/>
+      <c r="D58" s="51"/>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B59" s="31">
+      <c r="B59" s="24">
         <v>0.91666666666666696</v>
       </c>
-      <c r="C59" s="17" t="s">
+      <c r="C59" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D59" s="17" t="s">
+      <c r="D59" s="10" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B60" s="28"/>
+      <c r="B60" s="21"/>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B61" s="34" t="s">
+      <c r="B61" s="27" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B62" s="34" t="s">
+      <c r="B62" s="27" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B63" s="22" t="s">
+      <c r="B63" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C63" s="23" t="s">
+      <c r="C63" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="D63" s="23" t="s">
+      <c r="D63" s="16" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B64" s="5">
+      <c r="B64" s="50">
         <v>0.29166666666666702</v>
       </c>
-      <c r="C64" s="12" t="s">
+      <c r="C64" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D64" s="6"/>
+      <c r="D64" s="51"/>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B65" s="5"/>
-      <c r="C65" s="12" t="s">
+      <c r="B65" s="50"/>
+      <c r="C65" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D65" s="6"/>
+      <c r="D65" s="51"/>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B66" s="5"/>
-      <c r="C66" s="17" t="s">
+      <c r="B66" s="50"/>
+      <c r="C66" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="D66" s="6"/>
+      <c r="D66" s="51"/>
     </row>
     <row r="67" spans="2:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B67" s="1" t="s">
+      <c r="B67" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="C67" s="6" t="s">
+      <c r="C67" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="D67" s="12" t="s">
+      <c r="D67" s="5" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="68" spans="2:4" ht="45" x14ac:dyDescent="0.2">
-      <c r="B68" s="1"/>
-      <c r="C68" s="6"/>
-      <c r="D68" s="17" t="s">
+      <c r="B68" s="52"/>
+      <c r="C68" s="51"/>
+      <c r="D68" s="10" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B69" s="35">
+      <c r="B69" s="28">
         <v>0.36458333333333298</v>
       </c>
-      <c r="C69" s="17" t="s">
+      <c r="C69" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="D69" s="17"/>
+      <c r="D69" s="10"/>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B70" s="36"/>
-      <c r="C70" s="17" t="s">
+      <c r="B70" s="29"/>
+      <c r="C70" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="D70" s="17"/>
+      <c r="D70" s="10"/>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B71" s="36"/>
-      <c r="C71" s="17" t="s">
+      <c r="B71" s="29"/>
+      <c r="C71" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D71" s="17"/>
+      <c r="D71" s="10"/>
     </row>
     <row r="72" spans="2:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="B72" s="36"/>
-      <c r="C72" s="17" t="s">
+      <c r="B72" s="29"/>
+      <c r="C72" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="D72" s="17"/>
+      <c r="D72" s="10"/>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B73" s="36"/>
-      <c r="C73" s="17" t="s">
+      <c r="B73" s="29"/>
+      <c r="C73" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="D73" s="17"/>
+      <c r="D73" s="10"/>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B74" s="36"/>
-      <c r="C74" s="17" t="s">
+      <c r="B74" s="29"/>
+      <c r="C74" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="D74" s="17"/>
+      <c r="D74" s="10"/>
     </row>
     <row r="75" spans="2:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="B75" s="36"/>
-      <c r="C75" s="17" t="s">
+      <c r="B75" s="29"/>
+      <c r="C75" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="D75" s="17"/>
+      <c r="D75" s="10"/>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B76" s="35">
+      <c r="B76" s="28">
         <v>0.45833333333333298</v>
       </c>
-      <c r="C76" s="17" t="s">
+      <c r="C76" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="D76" s="17"/>
+      <c r="D76" s="10"/>
     </row>
     <row r="77" spans="2:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="B77" s="24">
+      <c r="B77" s="17">
         <v>0.5</v>
       </c>
-      <c r="C77" s="17" t="s">
+      <c r="C77" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D77" s="17"/>
+      <c r="D77" s="10"/>
     </row>
     <row r="78" spans="2:4" ht="45" x14ac:dyDescent="0.2">
-      <c r="B78" s="24">
+      <c r="B78" s="17">
         <v>0.104166666666667</v>
       </c>
-      <c r="C78" s="17" t="s">
+      <c r="C78" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="D78" s="17"/>
+      <c r="D78" s="10"/>
     </row>
     <row r="79" spans="2:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="B79" s="36"/>
-      <c r="C79" s="17" t="s">
+      <c r="B79" s="29"/>
+      <c r="C79" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D79" s="17"/>
+      <c r="D79" s="10"/>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B80" s="33"/>
-      <c r="C80" s="17"/>
-      <c r="D80" s="17"/>
+      <c r="B80" s="26"/>
+      <c r="C80" s="10"/>
+      <c r="D80" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="B26:B31"/>
+    <mergeCell ref="D26:D31"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="D46:D47"/>
     <mergeCell ref="B64:B66"/>
     <mergeCell ref="D64:D66"/>
     <mergeCell ref="B67:B68"/>
@@ -5000,23 +5035,6 @@
     <mergeCell ref="B57:B58"/>
     <mergeCell ref="C57:C58"/>
     <mergeCell ref="D57:D58"/>
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="B26:B31"/>
-    <mergeCell ref="D26:D31"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -5027,8 +5045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC91"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView topLeftCell="A94" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5053,55 +5071,55 @@
     <col min="19" max="1025" width="8.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="37" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:15" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="H1" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="I1" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="J1" s="37" t="s">
+      <c r="J1" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="K1" s="37" t="s">
+      <c r="K1" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="L1" s="37" t="s">
+      <c r="L1" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="M1" s="37" t="s">
+      <c r="M1" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="N1" s="37" t="s">
+      <c r="N1" s="30" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="13" t="s">
         <v>129</v>
       </c>
     </row>
@@ -5118,7 +5136,7 @@
       <c r="E3" t="s">
         <v>133</v>
       </c>
-      <c r="F3" s="38">
+      <c r="F3" s="31">
         <v>7</v>
       </c>
       <c r="G3" t="s">
@@ -5146,7 +5164,7 @@
       <c r="H5" t="s">
         <v>139</v>
       </c>
-      <c r="I5" s="39"/>
+      <c r="I5" s="32"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F6">
@@ -5155,7 +5173,7 @@
       <c r="H6" t="s">
         <v>140</v>
       </c>
-      <c r="I6" s="39" t="s">
+      <c r="I6" s="32" t="s">
         <v>140</v>
       </c>
       <c r="L6" t="s">
@@ -5218,7 +5236,7 @@
       <c r="I9" t="s">
         <v>155</v>
       </c>
-      <c r="J9" s="40" t="s">
+      <c r="J9" s="33" t="s">
         <v>156</v>
       </c>
       <c r="L9" t="s">
@@ -5273,34 +5291,34 @@
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="42" t="s">
+    <row r="15" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="35" t="s">
         <v>168</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="42"/>
-      <c r="B16" s="42" t="s">
+      <c r="A16" s="35"/>
+      <c r="B16" s="35" t="s">
         <v>171</v>
       </c>
       <c r="E16" t="s">
         <v>172</v>
       </c>
-      <c r="F16" s="44">
+      <c r="F16" s="37">
         <v>5</v>
       </c>
-      <c r="G16" s="45" t="s">
+      <c r="G16" s="38" t="s">
         <v>173</v>
       </c>
       <c r="J16" t="s">
@@ -5320,15 +5338,15 @@
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42" t="s">
+      <c r="A17" s="35"/>
+      <c r="B17" s="35" t="s">
         <v>179</v>
       </c>
       <c r="D17" t="s">
         <v>180</v>
       </c>
-      <c r="F17" s="45"/>
-      <c r="M17" s="46">
+      <c r="F17" s="38"/>
+      <c r="M17" s="39">
         <v>0.35416666666666702</v>
       </c>
       <c r="N17">
@@ -5339,8 +5357,8 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42" t="s">
+      <c r="A18" s="35"/>
+      <c r="B18" s="35" t="s">
         <v>182</v>
       </c>
       <c r="D18" t="s">
@@ -5349,10 +5367,10 @@
       <c r="E18" t="s">
         <v>184</v>
       </c>
-      <c r="F18" s="45">
+      <c r="F18" s="38">
         <v>1</v>
       </c>
-      <c r="G18" s="45" t="s">
+      <c r="G18" s="38" t="s">
         <v>185</v>
       </c>
       <c r="H18" t="s">
@@ -5361,7 +5379,7 @@
       <c r="L18" t="s">
         <v>187</v>
       </c>
-      <c r="M18" s="46">
+      <c r="M18" s="39">
         <v>0.45833333333333298</v>
       </c>
       <c r="N18">
@@ -5378,10 +5396,10 @@
       <c r="E19" t="s">
         <v>167</v>
       </c>
-      <c r="F19" s="45">
+      <c r="F19" s="38">
         <v>2</v>
       </c>
-      <c r="G19" s="45" t="s">
+      <c r="G19" s="38" t="s">
         <v>190</v>
       </c>
       <c r="H19" t="s">
@@ -5390,7 +5408,7 @@
       <c r="L19" t="s">
         <v>192</v>
       </c>
-      <c r="M19" s="46">
+      <c r="M19" s="39">
         <v>0.46666666666666701</v>
       </c>
       <c r="N19">
@@ -5404,10 +5422,10 @@
       <c r="D20" t="s">
         <v>194</v>
       </c>
-      <c r="F20" s="45">
+      <c r="F20" s="38">
         <v>3</v>
       </c>
-      <c r="G20" s="45" t="s">
+      <c r="G20" s="38" t="s">
         <v>195</v>
       </c>
       <c r="H20" t="s">
@@ -5416,7 +5434,7 @@
       <c r="L20" t="s">
         <v>197</v>
       </c>
-      <c r="M20" s="46">
+      <c r="M20" s="39">
         <v>0.54166666666666696</v>
       </c>
       <c r="N20">
@@ -5427,10 +5445,10 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F21" s="45">
+      <c r="F21" s="38">
         <v>4</v>
       </c>
-      <c r="G21" s="45" t="s">
+      <c r="G21" s="38" t="s">
         <v>195</v>
       </c>
       <c r="H21" t="s">
@@ -5439,7 +5457,7 @@
       <c r="I21" t="s">
         <v>200</v>
       </c>
-      <c r="M21" s="46">
+      <c r="M21" s="39">
         <v>0.54513888888888895</v>
       </c>
       <c r="N21">
@@ -5450,16 +5468,16 @@
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F22" s="45">
+      <c r="F22" s="38">
         <v>5</v>
       </c>
-      <c r="G22" s="45" t="s">
+      <c r="G22" s="38" t="s">
         <v>202</v>
       </c>
       <c r="H22" t="s">
         <v>203</v>
       </c>
-      <c r="M22" s="46">
+      <c r="M22" s="39">
         <v>0.54861111111111105</v>
       </c>
       <c r="N22">
@@ -5470,16 +5488,16 @@
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F23" s="45">
+      <c r="F23" s="38">
         <v>6</v>
       </c>
-      <c r="G23" s="45" t="s">
+      <c r="G23" s="38" t="s">
         <v>202</v>
       </c>
       <c r="H23" t="s">
         <v>205</v>
       </c>
-      <c r="M23" s="46">
+      <c r="M23" s="39">
         <v>0.70833333333333304</v>
       </c>
       <c r="N23">
@@ -5490,13 +5508,13 @@
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F24" s="45">
+      <c r="F24" s="38">
         <v>7</v>
       </c>
-      <c r="G24" s="45" t="s">
+      <c r="G24" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="M24" s="46">
+      <c r="M24" s="39">
         <v>0.71666666666666701</v>
       </c>
       <c r="N24">
@@ -5507,13 +5525,13 @@
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F25" s="45">
+      <c r="F25" s="38">
         <v>8</v>
       </c>
-      <c r="G25" s="45" t="s">
+      <c r="G25" s="38" t="s">
         <v>207</v>
       </c>
-      <c r="M25" s="46">
+      <c r="M25" s="39">
         <v>0.79166666666666696</v>
       </c>
       <c r="N25">
@@ -5524,8 +5542,8 @@
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F26" s="45"/>
-      <c r="M26" s="46">
+      <c r="F26" s="38"/>
+      <c r="M26" s="39">
         <v>0.79513888888888895</v>
       </c>
       <c r="N26">
@@ -5542,11 +5560,11 @@
       <c r="E27" t="s">
         <v>209</v>
       </c>
-      <c r="F27" s="45"/>
-      <c r="I27" s="45" t="s">
+      <c r="F27" s="38"/>
+      <c r="I27" s="38" t="s">
         <v>210</v>
       </c>
-      <c r="M27" s="46">
+      <c r="M27" s="39">
         <v>0.79861111111111105</v>
       </c>
       <c r="N27">
@@ -5563,40 +5581,40 @@
       <c r="E28" t="s">
         <v>209</v>
       </c>
-      <c r="F28" s="45"/>
-      <c r="I28" s="45" t="s">
+      <c r="F28" s="38"/>
+      <c r="I28" s="38" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="30" spans="1:15" s="37" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="37" t="s">
+    <row r="30" spans="1:15" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="30" t="s">
         <v>216</v>
       </c>
-      <c r="B30" s="37" t="s">
+      <c r="B30" s="30" t="s">
         <v>217</v>
       </c>
-      <c r="C30" s="37" t="s">
+      <c r="C30" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="D30" s="37" t="s">
+      <c r="D30" s="30" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B31" s="37" t="s">
+      <c r="B31" s="30" t="s">
         <v>219</v>
       </c>
-      <c r="C31" s="37" t="s">
+      <c r="C31" s="30" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B33" s="37" t="s">
+      <c r="B33" s="30" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B34" s="37" t="s">
+      <c r="B34" s="30" t="s">
         <v>222</v>
       </c>
       <c r="D34" t="s">
@@ -5605,7 +5623,7 @@
       <c r="E34" t="s">
         <v>133</v>
       </c>
-      <c r="F34" s="38">
+      <c r="F34" s="31">
         <v>10</v>
       </c>
       <c r="G34" t="s">
@@ -5616,7 +5634,7 @@
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B35" s="37" t="s">
+      <c r="B35" s="30" t="s">
         <v>224</v>
       </c>
       <c r="D35" t="s">
@@ -5627,7 +5645,7 @@
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B36" s="37" t="s">
+      <c r="B36" s="30" t="s">
         <v>226</v>
       </c>
       <c r="F36">
@@ -5636,7 +5654,7 @@
       <c r="H36" t="s">
         <v>139</v>
       </c>
-      <c r="I36" s="39"/>
+      <c r="I36" s="32"/>
       <c r="N36" t="s">
         <v>142</v>
       </c>
@@ -5657,7 +5675,7 @@
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B37" s="37" t="s">
+      <c r="B37" s="30" t="s">
         <v>230</v>
       </c>
       <c r="F37">
@@ -5671,7 +5689,7 @@
       </c>
     </row>
     <row r="38" spans="1:19" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="37" t="s">
+      <c r="B38" s="30" t="s">
         <v>231</v>
       </c>
       <c r="F38">
@@ -5774,7 +5792,7 @@
       <c r="I43" t="s">
         <v>155</v>
       </c>
-      <c r="J43" s="40" t="s">
+      <c r="J43" s="33" t="s">
         <v>156</v>
       </c>
       <c r="L43" t="s">
@@ -5821,37 +5839,37 @@
         <v>161</v>
       </c>
     </row>
-    <row r="47" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="37" t="s">
+    <row r="47" spans="1:19" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="30" t="s">
         <v>216</v>
       </c>
-      <c r="B47" s="37" t="s">
+      <c r="B47" s="30" t="s">
         <v>244</v>
       </c>
-      <c r="C47" s="37" t="s">
+      <c r="C47" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="D47" s="37" t="s">
+      <c r="D47" s="30" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B48" s="37" t="s">
+      <c r="B48" s="30" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="49" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B49" s="37" t="s">
+      <c r="B49" s="30" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="50" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B50" s="37" t="s">
+      <c r="B50" s="30" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="51" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B51" s="37" t="s">
+      <c r="B51" s="30" t="s">
         <v>250</v>
       </c>
     </row>
@@ -5862,7 +5880,7 @@
       <c r="E52" t="s">
         <v>133</v>
       </c>
-      <c r="F52" s="38">
+      <c r="F52" s="31">
         <v>15</v>
       </c>
       <c r="G52" t="s">
@@ -5887,7 +5905,7 @@
       <c r="H54" t="s">
         <v>139</v>
       </c>
-      <c r="I54" s="39"/>
+      <c r="I54" s="32"/>
       <c r="N54" t="s">
         <v>254</v>
       </c>
@@ -6007,7 +6025,7 @@
       <c r="I61" t="s">
         <v>155</v>
       </c>
-      <c r="J61" s="41" t="s">
+      <c r="J61" s="34" t="s">
         <v>258</v>
       </c>
       <c r="L61" t="s">
@@ -6064,7 +6082,7 @@
       <c r="I64" t="s">
         <v>260</v>
       </c>
-      <c r="J64" s="41" t="s">
+      <c r="J64" s="34" t="s">
         <v>261</v>
       </c>
       <c r="L64" t="s">
@@ -6081,7 +6099,7 @@
       <c r="I65" t="s">
         <v>264</v>
       </c>
-      <c r="J65" s="41" t="s">
+      <c r="J65" s="34" t="s">
         <v>261</v>
       </c>
     </row>
@@ -6095,7 +6113,7 @@
       <c r="I66" t="s">
         <v>266</v>
       </c>
-      <c r="J66" s="41" t="s">
+      <c r="J66" s="34" t="s">
         <v>261</v>
       </c>
     </row>
@@ -6109,7 +6127,7 @@
       <c r="I67" t="s">
         <v>268</v>
       </c>
-      <c r="J67" s="41" t="s">
+      <c r="J67" s="34" t="s">
         <v>261</v>
       </c>
     </row>
@@ -6123,33 +6141,33 @@
       <c r="I68" t="s">
         <v>268</v>
       </c>
-      <c r="J68" s="41" t="s">
+      <c r="J68" s="34" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="71" spans="4:29" x14ac:dyDescent="0.2">
-      <c r="D71" s="28" t="s">
+      <c r="D71" s="21" t="s">
         <v>270</v>
       </c>
       <c r="E71" t="s">
         <v>133</v>
       </c>
-      <c r="F71" s="47" t="s">
+      <c r="F71" s="40" t="s">
         <v>271</v>
       </c>
       <c r="I71" t="s">
         <v>272</v>
       </c>
-      <c r="J71" s="40"/>
+      <c r="J71" s="33"/>
     </row>
     <row r="72" spans="4:29" x14ac:dyDescent="0.2">
-      <c r="D72" s="28" t="s">
+      <c r="D72" s="21" t="s">
         <v>273</v>
       </c>
       <c r="E72" t="s">
         <v>138</v>
       </c>
-      <c r="F72" s="47" t="s">
+      <c r="F72" s="40" t="s">
         <v>271</v>
       </c>
     </row>
@@ -6160,7 +6178,7 @@
       <c r="E73" t="s">
         <v>215</v>
       </c>
-      <c r="F73" s="47" t="s">
+      <c r="F73" s="40" t="s">
         <v>271</v>
       </c>
       <c r="I73" t="s">
@@ -6222,7 +6240,7 @@
       <c r="E75" t="s">
         <v>133</v>
       </c>
-      <c r="F75" s="47" t="s">
+      <c r="F75" s="40" t="s">
         <v>293</v>
       </c>
       <c r="L75" t="s">
@@ -6242,7 +6260,7 @@
       <c r="E76" t="s">
         <v>167</v>
       </c>
-      <c r="F76" s="47" t="s">
+      <c r="F76" s="40" t="s">
         <v>293</v>
       </c>
     </row>
@@ -6253,13 +6271,13 @@
       <c r="E77" t="s">
         <v>133</v>
       </c>
-      <c r="F77" s="47" t="s">
+      <c r="F77" s="40" t="s">
         <v>293</v>
       </c>
-      <c r="I77" s="40" t="s">
+      <c r="I77" s="33" t="s">
         <v>156</v>
       </c>
-      <c r="J77" s="40" t="s">
+      <c r="J77" s="33" t="s">
         <v>156</v>
       </c>
     </row>
@@ -6270,7 +6288,7 @@
       <c r="E78" t="s">
         <v>167</v>
       </c>
-      <c r="F78" s="47" t="s">
+      <c r="F78" s="40" t="s">
         <v>293</v>
       </c>
     </row>
@@ -6303,7 +6321,7 @@
       <c r="I81" t="s">
         <v>268</v>
       </c>
-      <c r="J81" s="40" t="s">
+      <c r="J81" s="33" t="s">
         <v>156</v>
       </c>
     </row>
@@ -6316,9 +6334,9 @@
       </c>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A83" s="48"/>
-      <c r="B83" s="48"/>
-      <c r="C83" s="48"/>
+      <c r="A83" s="41"/>
+      <c r="B83" s="41"/>
+      <c r="C83" s="41"/>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D84" t="s">
@@ -6327,7 +6345,7 @@
       <c r="E84" t="s">
         <v>133</v>
       </c>
-      <c r="F84" s="47" t="s">
+      <c r="F84" s="40" t="s">
         <v>293</v>
       </c>
       <c r="L84" t="s">
@@ -6347,7 +6365,7 @@
       <c r="E85" t="s">
         <v>167</v>
       </c>
-      <c r="F85" s="47" t="s">
+      <c r="F85" s="40" t="s">
         <v>293</v>
       </c>
     </row>
@@ -6358,13 +6376,13 @@
       <c r="E86" t="s">
         <v>133</v>
       </c>
-      <c r="F86" s="47" t="s">
+      <c r="F86" s="40" t="s">
         <v>293</v>
       </c>
-      <c r="I86" s="40" t="s">
+      <c r="I86" s="33" t="s">
         <v>156</v>
       </c>
-      <c r="J86" s="40" t="s">
+      <c r="J86" s="33" t="s">
         <v>156</v>
       </c>
     </row>
@@ -6375,7 +6393,7 @@
       <c r="E87" t="s">
         <v>167</v>
       </c>
-      <c r="F87" s="47" t="s">
+      <c r="F87" s="40" t="s">
         <v>293</v>
       </c>
     </row>
@@ -6386,7 +6404,7 @@
       <c r="E88" t="s">
         <v>133</v>
       </c>
-      <c r="F88" s="47" t="s">
+      <c r="F88" s="40" t="s">
         <v>293</v>
       </c>
       <c r="I88" t="s">
@@ -6400,7 +6418,7 @@
       <c r="E89" t="s">
         <v>167</v>
       </c>
-      <c r="F89" s="47" t="s">
+      <c r="F89" s="40" t="s">
         <v>293</v>
       </c>
     </row>
@@ -6411,13 +6429,13 @@
       <c r="E90" t="s">
         <v>133</v>
       </c>
-      <c r="F90" s="47" t="s">
+      <c r="F90" s="40" t="s">
         <v>293</v>
       </c>
       <c r="I90" t="s">
         <v>268</v>
       </c>
-      <c r="J90" s="40" t="s">
+      <c r="J90" s="33" t="s">
         <v>156</v>
       </c>
     </row>
@@ -6439,8 +6457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F445"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D303" sqref="D303"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6455,25 +6473,25 @@
     <col min="8" max="1025" width="8.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="35" t="s">
         <v>310</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="35" t="s">
         <v>311</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="35" t="s">
         <v>312</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="35" t="s">
         <v>313</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="E1" s="35" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="49" t="s">
+    <row r="2" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="42" t="s">
         <v>314</v>
       </c>
     </row>
@@ -6520,33 +6538,34 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="57" t="s">
         <v>325</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="57" t="s">
         <v>326</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="57" t="s">
         <v>327</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="57" t="s">
         <v>328</v>
       </c>
+      <c r="E6" s="57"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="60" t="s">
         <v>329</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="60">
         <v>60</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="60">
         <v>63</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="60" t="s">
         <v>330</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="60" t="s">
         <v>331</v>
       </c>
     </row>
@@ -6554,10 +6573,10 @@
       <c r="A8" t="s">
         <v>332</v>
       </c>
-      <c r="B8" s="50">
+      <c r="B8" s="43">
         <v>1.651</v>
       </c>
-      <c r="C8" s="50">
+      <c r="C8" s="43">
         <v>1.6002000000000001</v>
       </c>
       <c r="D8" t="s">
@@ -6571,10 +6590,10 @@
       <c r="A9" t="s">
         <v>335</v>
       </c>
-      <c r="B9" s="50">
+      <c r="B9" s="43">
         <v>63.502931799999999</v>
       </c>
-      <c r="C9" s="50">
+      <c r="C9" s="43">
         <v>53.977492030000001</v>
       </c>
       <c r="D9" t="s">
@@ -6585,32 +6604,34 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="60" t="s">
         <v>338</v>
       </c>
-      <c r="B10" s="50">
+      <c r="B10" s="61">
         <v>23.296980153723599</v>
       </c>
-      <c r="C10" s="50">
+      <c r="C10" s="61">
         <v>21.0796875729554</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="60" t="s">
         <v>339</v>
       </c>
+      <c r="E10" s="60"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="60" t="s">
         <v>340</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="60" t="s">
         <v>341</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="60" t="s">
         <v>341</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="60" t="s">
         <v>342</v>
       </c>
+      <c r="E11" s="60"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -6641,32 +6662,34 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="57" t="s">
         <v>350</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="57" t="s">
         <v>351</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="57" t="s">
         <v>352</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="57" t="s">
         <v>353</v>
       </c>
+      <c r="E14" s="57"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="57" t="s">
         <v>354</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="57" t="s">
         <v>355</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="57" t="s">
         <v>352</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="57" t="s">
         <v>356</v>
       </c>
+      <c r="E15" s="57"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -6721,10 +6744,10 @@
       <c r="A20" t="s">
         <v>363</v>
       </c>
-      <c r="B20" s="51" t="s">
+      <c r="B20" s="44" t="s">
         <v>323</v>
       </c>
-      <c r="C20" s="51" t="s">
+      <c r="C20" s="44" t="s">
         <v>323</v>
       </c>
       <c r="D20" t="str">
@@ -6736,10 +6759,10 @@
       <c r="A21" t="s">
         <v>364</v>
       </c>
-      <c r="B21" s="51">
+      <c r="B21" s="44">
         <v>15</v>
       </c>
-      <c r="C21" s="51"/>
+      <c r="C21" s="44"/>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
         <v>ALCOHOL Dose/Week</v>
@@ -6749,10 +6772,10 @@
       <c r="A22" t="s">
         <v>365</v>
       </c>
-      <c r="B22" s="51" t="s">
+      <c r="B22" s="44" t="s">
         <v>322</v>
       </c>
-      <c r="C22" s="51" t="s">
+      <c r="C22" s="44" t="s">
         <v>322</v>
       </c>
       <c r="D22" t="str">
@@ -6764,10 +6787,10 @@
       <c r="A23" t="s">
         <v>366</v>
       </c>
-      <c r="B23" s="51" t="s">
+      <c r="B23" s="44" t="s">
         <v>322</v>
       </c>
-      <c r="C23" s="51" t="s">
+      <c r="C23" s="44" t="s">
         <v>322</v>
       </c>
       <c r="D23" t="str">
@@ -6779,10 +6802,10 @@
       <c r="A24" t="s">
         <v>367</v>
       </c>
-      <c r="B24" s="51" t="s">
+      <c r="B24" s="44" t="s">
         <v>322</v>
       </c>
-      <c r="C24" s="51" t="s">
+      <c r="C24" s="44" t="s">
         <v>322</v>
       </c>
       <c r="D24" t="str">
@@ -6794,10 +6817,10 @@
       <c r="A25" t="s">
         <v>368</v>
       </c>
-      <c r="B25" s="51" t="s">
+      <c r="B25" s="44" t="s">
         <v>323</v>
       </c>
-      <c r="C25" s="51" t="s">
+      <c r="C25" s="44" t="s">
         <v>322</v>
       </c>
       <c r="D25" t="str">
@@ -6809,10 +6832,10 @@
       <c r="A26" t="s">
         <v>369</v>
       </c>
-      <c r="B26" s="51" t="s">
+      <c r="B26" s="44" t="s">
         <v>322</v>
       </c>
-      <c r="C26" s="51" t="s">
+      <c r="C26" s="44" t="s">
         <v>322</v>
       </c>
       <c r="D26" t="str">
@@ -6824,10 +6847,10 @@
       <c r="A27" t="s">
         <v>370</v>
       </c>
-      <c r="B27" s="51" t="s">
+      <c r="B27" s="44" t="s">
         <v>322</v>
       </c>
-      <c r="C27" s="51" t="s">
+      <c r="C27" s="44" t="s">
         <v>323</v>
       </c>
       <c r="D27" t="str">
@@ -6839,10 +6862,10 @@
       <c r="A28" t="s">
         <v>371</v>
       </c>
-      <c r="B28" s="51">
+      <c r="B28" s="44">
         <v>1</v>
       </c>
-      <c r="C28" s="51">
+      <c r="C28" s="44">
         <v>1</v>
       </c>
       <c r="D28" t="s">
@@ -6853,10 +6876,10 @@
       <c r="A29" t="s">
         <v>373</v>
       </c>
-      <c r="B29" s="51" t="s">
+      <c r="B29" s="44" t="s">
         <v>374</v>
       </c>
-      <c r="C29" s="51" t="s">
+      <c r="C29" s="44" t="s">
         <v>334</v>
       </c>
       <c r="D29" t="s">
@@ -6867,10 +6890,10 @@
       <c r="A30" t="s">
         <v>376</v>
       </c>
-      <c r="B30" s="51">
+      <c r="B30" s="44">
         <v>2</v>
       </c>
-      <c r="C30" s="51">
+      <c r="C30" s="44">
         <v>1</v>
       </c>
       <c r="D30" t="s">
@@ -6881,10 +6904,10 @@
       <c r="A31" t="s">
         <v>378</v>
       </c>
-      <c r="B31" s="51" t="s">
+      <c r="B31" s="44" t="s">
         <v>379</v>
       </c>
-      <c r="C31" s="51" t="s">
+      <c r="C31" s="44" t="s">
         <v>379</v>
       </c>
       <c r="D31" t="s">
@@ -6895,10 +6918,10 @@
       <c r="A32" t="s">
         <v>381</v>
       </c>
-      <c r="B32" s="51">
+      <c r="B32" s="44">
         <v>0</v>
       </c>
-      <c r="C32" s="51">
+      <c r="C32" s="44">
         <v>0</v>
       </c>
       <c r="D32" t="s">
@@ -6909,8 +6932,8 @@
       <c r="A33" t="s">
         <v>383</v>
       </c>
-      <c r="B33" s="51"/>
-      <c r="C33" s="51"/>
+      <c r="B33" s="44"/>
+      <c r="C33" s="44"/>
       <c r="D33" t="s">
         <v>384</v>
       </c>
@@ -6919,10 +6942,10 @@
       <c r="A34" t="s">
         <v>385</v>
       </c>
-      <c r="B34" s="51">
+      <c r="B34" s="44">
         <v>0</v>
       </c>
-      <c r="C34" s="51">
+      <c r="C34" s="44">
         <v>0</v>
       </c>
       <c r="D34" t="s">
@@ -6933,46 +6956,48 @@
       <c r="A35" t="s">
         <v>386</v>
       </c>
-      <c r="B35" s="51"/>
-      <c r="C35" s="51"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="44"/>
       <c r="D35" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="A36" s="57" t="s">
         <v>388</v>
       </c>
-      <c r="B36" s="51">
+      <c r="B36" s="59">
         <v>0</v>
       </c>
-      <c r="C36" s="51">
+      <c r="C36" s="59">
         <v>0</v>
       </c>
-      <c r="D36" t="str">
+      <c r="D36" s="57" t="str">
         <f>A36</f>
         <v>StrokeFAMILY HISTORY</v>
       </c>
+      <c r="E36" s="57"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="A37" s="57" t="s">
         <v>389</v>
       </c>
-      <c r="B37" s="51"/>
-      <c r="C37" s="51"/>
-      <c r="D37" t="str">
+      <c r="B37" s="59"/>
+      <c r="C37" s="59"/>
+      <c r="D37" s="57" t="str">
         <f>A37</f>
         <v>StrokeSpecific FAMILY HISTORY</v>
       </c>
+      <c r="E37" s="57"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>390</v>
       </c>
-      <c r="B38" s="51">
+      <c r="B38" s="44">
         <v>0</v>
       </c>
-      <c r="C38" s="51"/>
+      <c r="C38" s="44"/>
       <c r="D38" t="s">
         <v>391</v>
       </c>
@@ -6981,10 +7006,10 @@
       <c r="A39" t="s">
         <v>392</v>
       </c>
-      <c r="B39" s="51" t="s">
+      <c r="B39" s="44" t="s">
         <v>322</v>
       </c>
-      <c r="C39" s="51" t="s">
+      <c r="C39" s="44" t="s">
         <v>322</v>
       </c>
       <c r="D39" t="str">
@@ -6993,43 +7018,45 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="A40" s="57" t="s">
         <v>393</v>
       </c>
-      <c r="B40" s="51" t="s">
+      <c r="B40" s="59" t="s">
         <v>322</v>
       </c>
-      <c r="C40" s="51" t="s">
+      <c r="C40" s="59" t="s">
         <v>323</v>
       </c>
-      <c r="D40" t="str">
+      <c r="D40" s="57" t="str">
         <f t="shared" si="1"/>
         <v>STROKE PATIENT MEDICAL HISTORY</v>
       </c>
+      <c r="E40" s="57"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="A41" s="57" t="s">
         <v>394</v>
       </c>
-      <c r="B41" s="51" t="s">
+      <c r="B41" s="59" t="s">
         <v>395</v>
       </c>
-      <c r="C41" s="51">
+      <c r="C41" s="59">
         <v>11</v>
       </c>
-      <c r="D41" t="str">
+      <c r="D41" s="57" t="str">
         <f t="shared" si="1"/>
         <v>STROKE YR PATIENT MEDICAL HISTORY</v>
       </c>
+      <c r="E41" s="57"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>396</v>
       </c>
-      <c r="B42" s="51" t="s">
+      <c r="B42" s="44" t="s">
         <v>322</v>
       </c>
-      <c r="C42" s="51" t="s">
+      <c r="C42" s="44" t="s">
         <v>397</v>
       </c>
       <c r="D42" t="str">
@@ -7041,10 +7068,10 @@
       <c r="A43" t="s">
         <v>398</v>
       </c>
-      <c r="B43" s="51" t="s">
+      <c r="B43" s="44" t="s">
         <v>322</v>
       </c>
-      <c r="C43" s="51" t="s">
+      <c r="C43" s="44" t="s">
         <v>322</v>
       </c>
       <c r="D43" t="str">
@@ -7056,10 +7083,10 @@
       <c r="A44" t="s">
         <v>399</v>
       </c>
-      <c r="B44" s="51" t="s">
+      <c r="B44" s="44" t="s">
         <v>323</v>
       </c>
-      <c r="C44" s="51" t="s">
+      <c r="C44" s="44" t="s">
         <v>323</v>
       </c>
       <c r="D44" t="str">
@@ -7071,10 +7098,10 @@
       <c r="A45" t="s">
         <v>400</v>
       </c>
-      <c r="B45" s="51" t="s">
+      <c r="B45" s="44" t="s">
         <v>322</v>
       </c>
-      <c r="C45" s="51" t="s">
+      <c r="C45" s="44" t="s">
         <v>322</v>
       </c>
       <c r="D45" t="str">
@@ -7083,71 +7110,82 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="A46" s="57" t="s">
         <v>401</v>
       </c>
-      <c r="B46" s="51"/>
-      <c r="C46" s="51">
+      <c r="B46" s="59"/>
+      <c r="C46" s="59">
         <v>1994</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="57" t="s">
         <v>402</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="57" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="A47" s="57" t="s">
         <v>403</v>
       </c>
-      <c r="C47">
+      <c r="B47" s="57"/>
+      <c r="C47" s="57">
         <v>10</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="57" t="s">
         <v>404</v>
       </c>
-      <c r="E47" s="52"/>
+      <c r="E47" s="58"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+      <c r="A48" s="57" t="s">
         <v>405</v>
       </c>
-      <c r="C48">
+      <c r="B48" s="57"/>
+      <c r="C48" s="57">
         <v>3</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="57" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="E48" s="57"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="57" t="s">
         <v>407</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="57" t="s">
         <v>408</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="57" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="D49" s="57"/>
+      <c r="E49" s="57"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="57" t="s">
         <v>410</v>
       </c>
-      <c r="C50" t="s">
+      <c r="B50" s="57"/>
+      <c r="C50" s="57" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+      <c r="D50" s="57"/>
+      <c r="E50" s="57"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="57" t="s">
         <v>412</v>
       </c>
-      <c r="C51" t="s">
+      <c r="B51" s="57"/>
+      <c r="C51" s="57" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D51" s="57"/>
+      <c r="E51" s="57"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>414</v>
       </c>
@@ -7155,7 +7193,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>416</v>
       </c>
@@ -7166,7 +7204,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>419</v>
       </c>
@@ -7177,7 +7215,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>422</v>
       </c>
@@ -7191,7 +7229,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>425</v>
       </c>
@@ -7205,7 +7243,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>428</v>
       </c>
@@ -7219,7 +7257,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>430</v>
       </c>
@@ -7233,7 +7271,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>431</v>
       </c>
@@ -7247,7 +7285,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>432</v>
       </c>
@@ -7261,7 +7299,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>433</v>
       </c>
@@ -7275,7 +7313,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>434</v>
       </c>
@@ -7289,7 +7327,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>435</v>
       </c>
@@ -7303,7 +7341,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>436</v>
       </c>
@@ -9110,7 +9148,7 @@
       <c r="B174">
         <v>-0.62917567500000005</v>
       </c>
-      <c r="C174" s="40">
+      <c r="C174" s="33">
         <v>-0.28290422700000001</v>
       </c>
       <c r="D174" t="s">
@@ -9119,7 +9157,7 @@
       <c r="E174" t="s">
         <v>236</v>
       </c>
-      <c r="F174" s="40" t="s">
+      <c r="F174" s="33" t="s">
         <v>667</v>
       </c>
     </row>
@@ -9130,7 +9168,7 @@
       <c r="B175">
         <v>6.2716381160000001</v>
       </c>
-      <c r="C175" s="40">
+      <c r="C175" s="33">
         <v>-0.18184451800000001</v>
       </c>
       <c r="D175" t="s">
@@ -9139,7 +9177,7 @@
       <c r="E175" t="s">
         <v>236</v>
       </c>
-      <c r="F175" s="40" t="s">
+      <c r="F175" s="33" t="s">
         <v>667</v>
       </c>
     </row>
@@ -9255,7 +9293,7 @@
       <c r="B182">
         <v>44.396857199999999</v>
       </c>
-      <c r="C182" s="40">
+      <c r="C182" s="33">
         <v>-29.160308409999999</v>
       </c>
       <c r="D182" t="s">
@@ -9264,7 +9302,7 @@
       <c r="E182" t="s">
         <v>236</v>
       </c>
-      <c r="F182" s="40" t="s">
+      <c r="F182" s="33" t="s">
         <v>667</v>
       </c>
     </row>
@@ -9275,7 +9313,7 @@
       <c r="B183">
         <v>63.078681570000001</v>
       </c>
-      <c r="C183" s="40">
+      <c r="C183" s="33">
         <v>-6.8294767380000003</v>
       </c>
       <c r="D183" t="s">
@@ -9595,7 +9633,7 @@
       <c r="B202">
         <v>5.5309639410000004</v>
       </c>
-      <c r="C202" s="40">
+      <c r="C202" s="33">
         <v>-0.28516630700000001</v>
       </c>
       <c r="D202" t="s">
@@ -9604,7 +9642,7 @@
       <c r="E202" t="s">
         <v>236</v>
       </c>
-      <c r="F202" s="40" t="s">
+      <c r="F202" s="33" t="s">
         <v>667</v>
       </c>
     </row>
@@ -9615,7 +9653,7 @@
       <c r="B203">
         <v>11.77686065</v>
       </c>
-      <c r="C203" s="40">
+      <c r="C203" s="33">
         <v>-0.22152102600000001</v>
       </c>
       <c r="D203" t="s">
@@ -9624,7 +9662,7 @@
       <c r="E203" t="s">
         <v>236</v>
       </c>
-      <c r="F203" s="40" t="s">
+      <c r="F203" s="33" t="s">
         <v>667</v>
       </c>
     </row>
@@ -10493,7 +10531,7 @@
       <c r="C269">
         <v>52</v>
       </c>
-      <c r="D269" s="8" t="s">
+      <c r="D269" s="1" t="s">
         <v>822</v>
       </c>
     </row>
@@ -10507,7 +10545,7 @@
       <c r="C270">
         <v>35</v>
       </c>
-      <c r="D270" s="8" t="s">
+      <c r="D270" s="1" t="s">
         <v>822</v>
       </c>
     </row>
@@ -10521,7 +10559,7 @@
       <c r="C271">
         <v>35</v>
       </c>
-      <c r="D271" s="8" t="s">
+      <c r="D271" s="1" t="s">
         <v>822</v>
       </c>
     </row>
@@ -10535,7 +10573,7 @@
       <c r="C272">
         <v>219</v>
       </c>
-      <c r="D272" s="8" t="s">
+      <c r="D272" s="1" t="s">
         <v>822</v>
       </c>
     </row>
@@ -10549,7 +10587,7 @@
       <c r="C273">
         <v>22</v>
       </c>
-      <c r="D273" s="8" t="s">
+      <c r="D273" s="1" t="s">
         <v>822</v>
       </c>
     </row>
@@ -10563,7 +10601,7 @@
       <c r="C274">
         <v>205</v>
       </c>
-      <c r="D274" s="8" t="s">
+      <c r="D274" s="1" t="s">
         <v>822</v>
       </c>
     </row>
@@ -10577,7 +10615,7 @@
       <c r="C275">
         <v>61</v>
       </c>
-      <c r="D275" s="8" t="s">
+      <c r="D275" s="1" t="s">
         <v>822</v>
       </c>
     </row>
@@ -10591,7 +10629,7 @@
       <c r="C276">
         <v>86</v>
       </c>
-      <c r="D276" s="8" t="s">
+      <c r="D276" s="1" t="s">
         <v>822</v>
       </c>
     </row>
@@ -10605,7 +10643,7 @@
       <c r="C277">
         <v>22</v>
       </c>
-      <c r="D277" s="8" t="s">
+      <c r="D277" s="1" t="s">
         <v>822</v>
       </c>
     </row>
@@ -10619,7 +10657,7 @@
       <c r="C278">
         <v>177</v>
       </c>
-      <c r="D278" s="8" t="s">
+      <c r="D278" s="1" t="s">
         <v>822</v>
       </c>
     </row>
@@ -10633,7 +10671,7 @@
       <c r="C279">
         <v>62</v>
       </c>
-      <c r="D279" s="8" t="s">
+      <c r="D279" s="1" t="s">
         <v>822</v>
       </c>
     </row>
@@ -10647,7 +10685,7 @@
       <c r="C280">
         <v>88</v>
       </c>
-      <c r="D280" s="8" t="s">
+      <c r="D280" s="1" t="s">
         <v>822</v>
       </c>
     </row>
@@ -10661,7 +10699,7 @@
       <c r="C281">
         <v>7</v>
       </c>
-      <c r="D281" s="8" t="s">
+      <c r="D281" s="1" t="s">
         <v>822</v>
       </c>
     </row>
@@ -10675,7 +10713,7 @@
       <c r="C282">
         <v>17</v>
       </c>
-      <c r="D282" s="8" t="s">
+      <c r="D282" s="1" t="s">
         <v>822</v>
       </c>
     </row>
@@ -10689,7 +10727,7 @@
       <c r="C283">
         <v>0</v>
       </c>
-      <c r="D283" s="8" t="s">
+      <c r="D283" s="1" t="s">
         <v>822</v>
       </c>
     </row>
@@ -10703,7 +10741,7 @@
       <c r="C284">
         <v>17</v>
       </c>
-      <c r="D284" s="8" t="s">
+      <c r="D284" s="1" t="s">
         <v>822</v>
       </c>
     </row>
@@ -10717,7 +10755,7 @@
       <c r="C285">
         <v>12</v>
       </c>
-      <c r="D285" s="8" t="s">
+      <c r="D285" s="1" t="s">
         <v>822</v>
       </c>
     </row>
@@ -10731,7 +10769,7 @@
       <c r="C286">
         <v>17</v>
       </c>
-      <c r="D286" s="8" t="s">
+      <c r="D286" s="1" t="s">
         <v>822</v>
       </c>
     </row>
@@ -10745,7 +10783,7 @@
       <c r="C287">
         <v>5</v>
       </c>
-      <c r="D287" s="8" t="s">
+      <c r="D287" s="1" t="s">
         <v>822</v>
       </c>
     </row>
@@ -10759,7 +10797,7 @@
       <c r="C288">
         <v>13.5</v>
       </c>
-      <c r="D288" s="8" t="s">
+      <c r="D288" s="1" t="s">
         <v>822</v>
       </c>
     </row>
@@ -10773,7 +10811,7 @@
       <c r="C289">
         <v>19</v>
       </c>
-      <c r="D289" s="8" t="s">
+      <c r="D289" s="1" t="s">
         <v>822</v>
       </c>
     </row>
@@ -10927,7 +10965,7 @@
       <c r="C300">
         <v>63</v>
       </c>
-      <c r="D300" s="8" t="s">
+      <c r="D300" s="1" t="s">
         <v>855</v>
       </c>
     </row>
@@ -10941,7 +10979,7 @@
       <c r="C301">
         <v>175</v>
       </c>
-      <c r="D301" s="8" t="s">
+      <c r="D301" s="1" t="s">
         <v>855</v>
       </c>
     </row>
@@ -10955,7 +10993,7 @@
       <c r="C302">
         <v>5</v>
       </c>
-      <c r="D302" s="8" t="s">
+      <c r="D302" s="1" t="s">
         <v>855</v>
       </c>
     </row>
@@ -10969,7 +11007,7 @@
       <c r="C303">
         <v>25</v>
       </c>
-      <c r="D303" s="8" t="s">
+      <c r="D303" s="1" t="s">
         <v>855</v>
       </c>
     </row>
@@ -10983,7 +11021,7 @@
       <c r="C304">
         <v>3</v>
       </c>
-      <c r="D304" s="8" t="s">
+      <c r="D304" s="1" t="s">
         <v>860</v>
       </c>
     </row>
@@ -10997,7 +11035,7 @@
       <c r="C305">
         <v>4</v>
       </c>
-      <c r="D305" s="8" t="s">
+      <c r="D305" s="1" t="s">
         <v>860</v>
       </c>
     </row>
@@ -11011,7 +11049,7 @@
       <c r="C306">
         <v>7</v>
       </c>
-      <c r="D306" s="8" t="s">
+      <c r="D306" s="1" t="s">
         <v>860</v>
       </c>
     </row>
@@ -11019,7 +11057,7 @@
       <c r="A307" t="s">
         <v>863</v>
       </c>
-      <c r="D307" s="8" t="s">
+      <c r="D307" s="1" t="s">
         <v>864</v>
       </c>
     </row>
@@ -11033,7 +11071,7 @@
       <c r="C308">
         <v>32</v>
       </c>
-      <c r="D308" s="8" t="s">
+      <c r="D308" s="1" t="s">
         <v>864</v>
       </c>
     </row>
@@ -11047,7 +11085,7 @@
       <c r="C309">
         <v>99</v>
       </c>
-      <c r="D309" s="8" t="s">
+      <c r="D309" s="1" t="s">
         <v>864</v>
       </c>
     </row>
@@ -11055,7 +11093,7 @@
       <c r="A310" t="s">
         <v>867</v>
       </c>
-      <c r="D310" s="8" t="s">
+      <c r="D310" s="1" t="s">
         <v>868</v>
       </c>
     </row>
@@ -11069,7 +11107,7 @@
       <c r="C311">
         <v>24</v>
       </c>
-      <c r="D311" s="8" t="s">
+      <c r="D311" s="1" t="s">
         <v>870</v>
       </c>
     </row>
@@ -11083,7 +11121,7 @@
       <c r="C312">
         <v>10</v>
       </c>
-      <c r="D312" s="8" t="s">
+      <c r="D312" s="1" t="s">
         <v>872</v>
       </c>
     </row>
@@ -11097,7 +11135,7 @@
       <c r="C313">
         <v>3</v>
       </c>
-      <c r="D313" s="8" t="s">
+      <c r="D313" s="1" t="s">
         <v>874</v>
       </c>
     </row>
@@ -12887,116 +12925,116 @@
         <v>Sleep(stability_results)</v>
       </c>
     </row>
-    <row r="436" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A436" s="53" t="s">
+    <row r="436" spans="1:4" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A436" s="45" t="s">
         <v>1021</v>
       </c>
-      <c r="B436" s="53">
+      <c r="B436" s="45">
         <v>0</v>
       </c>
-      <c r="C436" s="53">
+      <c r="C436" s="45">
         <v>0</v>
       </c>
-      <c r="D436" s="53" t="s">
+      <c r="D436" s="45" t="s">
         <v>1022</v>
       </c>
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A437" s="53" t="s">
+      <c r="A437" s="45" t="s">
         <v>1023</v>
       </c>
-      <c r="B437" s="53">
+      <c r="B437" s="45">
         <v>0</v>
       </c>
-      <c r="C437" s="53">
+      <c r="C437" s="45">
         <v>0</v>
       </c>
     </row>
     <row r="438" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A438" s="53" t="s">
+      <c r="A438" s="45" t="s">
         <v>1024</v>
       </c>
-      <c r="B438" s="53">
+      <c r="B438" s="45">
         <v>0</v>
       </c>
-      <c r="C438" s="53">
+      <c r="C438" s="45">
         <v>0</v>
       </c>
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A439" s="53" t="s">
+      <c r="A439" s="45" t="s">
         <v>1025</v>
       </c>
-      <c r="B439" s="53">
+      <c r="B439" s="45">
         <v>0</v>
       </c>
-      <c r="C439" s="53">
+      <c r="C439" s="45">
         <v>0</v>
       </c>
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A440" s="53" t="s">
+      <c r="A440" s="45" t="s">
         <v>1026</v>
       </c>
-      <c r="B440" s="53">
+      <c r="B440" s="45">
         <v>0</v>
       </c>
-      <c r="C440" s="53">
+      <c r="C440" s="45">
         <v>0</v>
       </c>
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A441" s="53" t="s">
+      <c r="A441" s="45" t="s">
         <v>1027</v>
       </c>
-      <c r="B441" s="53">
+      <c r="B441" s="45">
         <v>0</v>
       </c>
-      <c r="C441" s="53">
+      <c r="C441" s="45">
         <v>0</v>
       </c>
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A442" s="53" t="s">
+      <c r="A442" s="45" t="s">
         <v>1028</v>
       </c>
-      <c r="B442" s="53">
+      <c r="B442" s="45">
         <v>1</v>
       </c>
-      <c r="C442" s="53">
+      <c r="C442" s="45">
         <v>1</v>
       </c>
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A443" s="53" t="s">
+      <c r="A443" s="45" t="s">
         <v>1029</v>
       </c>
-      <c r="B443" s="53">
+      <c r="B443" s="45">
         <v>2</v>
       </c>
-      <c r="C443" s="53">
+      <c r="C443" s="45">
         <v>3</v>
       </c>
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A444" s="53" t="s">
+      <c r="A444" s="45" t="s">
         <v>1030</v>
       </c>
-      <c r="B444" s="53">
+      <c r="B444" s="45">
         <v>1</v>
       </c>
-      <c r="C444" s="53">
+      <c r="C444" s="45">
         <v>1</v>
       </c>
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A445" s="53" t="s">
+      <c r="A445" s="45" t="s">
         <v>1031</v>
       </c>
-      <c r="B445" s="53">
+      <c r="B445" s="45">
         <v>0</v>
       </c>
-      <c r="C445" s="53">
+      <c r="C445" s="45">
         <v>0</v>
       </c>
     </row>
@@ -13010,8 +13048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:M47"/>
   <sheetViews>
-    <sheetView zoomScale="157" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="A91" zoomScale="157" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13020,92 +13058,92 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="21" t="s">
         <v>1032</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="21" t="s">
         <v>1033</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="21" t="s">
         <v>1034</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="28"/>
+      <c r="A5" s="21"/>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="21" t="s">
         <v>1035</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="21" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="21" t="s">
         <v>1036</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="28"/>
+      <c r="A9" s="21"/>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="1" t="s">
         <v>1037</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="54" t="s">
+      <c r="A12" s="46" t="s">
         <v>1038</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="55" t="s">
+      <c r="A16" s="47" t="s">
         <v>1039</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="56" t="s">
+      <c r="A17" s="48" t="s">
         <v>1040</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="56" t="s">
+      <c r="A18" s="48" t="s">
         <v>1041</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="57" t="s">
+      <c r="A19" s="49" t="s">
         <v>1042</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A43" s="48" t="s">
+      <c r="A43" s="41" t="s">
         <v>1043</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A46" s="20" t="s">
+      <c r="A46" s="13" t="s">
         <v>1044</v>
       </c>
-      <c r="B46" s="20"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
-      <c r="G46" s="20"/>
-      <c r="H46" s="20"/>
-      <c r="I46" s="20"/>
-      <c r="J46" s="20"/>
-      <c r="K46" s="20"/>
-      <c r="L46" s="20"/>
-      <c r="M46" s="20"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="13"/>
+      <c r="K46" s="13"/>
+      <c r="L46" s="13"/>
+      <c r="M46" s="13"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">

</xml_diff>

<commit_message>
[ng-anhhtuann] Redefine model and labeling
</commit_message>
<xml_diff>
--- a/elderly-stroke/files-and-variables.xlsx
+++ b/elderly-stroke/files-and-variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macad/Documents/University/Thesis/ECG Processing/elderly-stroke/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466DA842-181F-FA4C-8DC0-DAA41A7CD064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B553AA29-3F9E-C245-BB31-877444C4BBB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="520" windowWidth="38400" windowHeight="21100" tabRatio="993" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="993" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Protocol and timeline" sheetId="1" r:id="rId1"/>
@@ -3562,7 +3562,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3596,12 +3596,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3715,7 +3709,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3828,17 +3822,17 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="7"/>
     </xf>
-    <xf numFmtId="18" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="18" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3846,14 +3840,17 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -4307,15 +4304,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -4323,22 +4320,22 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="51" t="s">
+      <c r="D4" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="51" t="s">
+      <c r="E4" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="54" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -4346,12 +4343,12 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="51"/>
-      <c r="B5" s="51"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" ht="51.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4507,18 +4504,18 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="50">
+      <c r="B20" s="55">
         <v>0.29166666666666702</v>
       </c>
-      <c r="C20" s="51" t="s">
+      <c r="C20" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="51"/>
+      <c r="D20" s="54"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B21" s="50"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="51"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="54"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B22" s="17">
@@ -4559,53 +4556,53 @@
       <c r="D25" s="10"/>
     </row>
     <row r="26" spans="1:5" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="54">
+      <c r="B26" s="56">
         <v>0.33333333333333298</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="51" t="s">
+      <c r="D26" s="54" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="B27" s="54"/>
+      <c r="B27" s="56"/>
       <c r="C27" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="51"/>
+      <c r="D27" s="54"/>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="B28" s="54"/>
+      <c r="B28" s="56"/>
       <c r="C28" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D28" s="51"/>
+      <c r="D28" s="54"/>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="B29" s="54"/>
+      <c r="B29" s="56"/>
       <c r="C29" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="51"/>
+      <c r="D29" s="54"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B30" s="54"/>
+      <c r="B30" s="56"/>
       <c r="C30" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D30" s="51"/>
+      <c r="D30" s="54"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B31" s="54"/>
+      <c r="B31" s="56"/>
       <c r="C31" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D31" s="51"/>
+      <c r="D31" s="54"/>
     </row>
     <row r="32" spans="1:5" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="54">
+      <c r="B32" s="56">
         <v>0.35416666666666702</v>
       </c>
       <c r="C32" s="5" t="s">
@@ -4617,14 +4614,14 @@
       <c r="E32" s="21"/>
     </row>
     <row r="33" spans="2:4" ht="55.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="54"/>
+      <c r="B33" s="56"/>
       <c r="C33" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D33" s="5"/>
     </row>
     <row r="34" spans="2:4" ht="55.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="54"/>
+      <c r="B34" s="56"/>
       <c r="C34" s="5" t="s">
         <v>53</v>
       </c>
@@ -4633,7 +4630,7 @@
       </c>
     </row>
     <row r="35" spans="2:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="B35" s="54"/>
+      <c r="B35" s="56"/>
       <c r="C35" s="5" t="s">
         <v>60</v>
       </c>
@@ -4642,21 +4639,21 @@
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B36" s="54"/>
+      <c r="B36" s="56"/>
       <c r="C36" s="22" t="s">
         <v>62</v>
       </c>
       <c r="D36" s="6"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B37" s="54"/>
+      <c r="B37" s="56"/>
       <c r="C37" s="22" t="s">
         <v>63</v>
       </c>
       <c r="D37" s="6"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B38" s="54"/>
+      <c r="B38" s="56"/>
       <c r="C38" s="23" t="s">
         <v>64</v>
       </c>
@@ -4685,7 +4682,7 @@
       </c>
     </row>
     <row r="41" spans="2:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="55">
+      <c r="B41" s="57">
         <v>0.47916666666666702</v>
       </c>
       <c r="C41" s="5" t="s">
@@ -4696,7 +4693,7 @@
       </c>
     </row>
     <row r="42" spans="2:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="55"/>
+      <c r="B42" s="57"/>
       <c r="C42" s="5" t="s">
         <v>71</v>
       </c>
@@ -4705,7 +4702,7 @@
       </c>
     </row>
     <row r="43" spans="2:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="B43" s="55"/>
+      <c r="B43" s="57"/>
       <c r="C43" s="6"/>
       <c r="D43" s="5" t="s">
         <v>73</v>
@@ -4714,7 +4711,7 @@
     <row r="44" spans="2:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="4"/>
       <c r="C44" s="5"/>
-      <c r="D44" s="51" t="s">
+      <c r="D44" s="54" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4725,57 +4722,57 @@
       <c r="C45" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="D45" s="51"/>
+      <c r="D45" s="54"/>
     </row>
     <row r="46" spans="2:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="53">
+      <c r="B46" s="58">
         <v>0.54166666666666696</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D46" s="51" t="s">
+      <c r="D46" s="54" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="48.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="53"/>
+      <c r="B47" s="58"/>
       <c r="C47" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D47" s="51"/>
+      <c r="D47" s="54"/>
     </row>
     <row r="48" spans="2:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="51" t="s">
+      <c r="B48" s="54" t="s">
         <v>78</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D48" s="51" t="s">
+      <c r="D48" s="54" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B49" s="51"/>
+      <c r="B49" s="54"/>
       <c r="C49" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D49" s="51"/>
+      <c r="D49" s="54"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B50" s="51"/>
+      <c r="B50" s="54"/>
       <c r="C50" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D50" s="51"/>
+      <c r="D50" s="54"/>
     </row>
     <row r="51" spans="2:4" ht="45" x14ac:dyDescent="0.2">
-      <c r="B51" s="51"/>
+      <c r="B51" s="54"/>
       <c r="C51" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="D51" s="51"/>
+      <c r="D51" s="54"/>
     </row>
     <row r="52" spans="2:4" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="26"/>
@@ -4787,7 +4784,7 @@
       </c>
     </row>
     <row r="53" spans="2:4" ht="41.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="53">
+      <c r="B53" s="58">
         <v>0.66666666666666696</v>
       </c>
       <c r="C53" s="5" t="s">
@@ -4798,7 +4795,7 @@
       </c>
     </row>
     <row r="54" spans="2:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="53"/>
+      <c r="B54" s="58"/>
       <c r="C54" s="5" t="s">
         <v>77</v>
       </c>
@@ -4807,7 +4804,7 @@
       </c>
     </row>
     <row r="55" spans="2:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="B55" s="53"/>
+      <c r="B55" s="58"/>
       <c r="C55" s="10" t="s">
         <v>88</v>
       </c>
@@ -4825,20 +4822,20 @@
       </c>
     </row>
     <row r="57" spans="2:4" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="53">
+      <c r="B57" s="58">
         <v>0.79166666666666696</v>
       </c>
-      <c r="C57" s="51" t="s">
+      <c r="C57" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="D57" s="51" t="s">
+      <c r="D57" s="54" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B58" s="53"/>
-      <c r="C58" s="51"/>
-      <c r="D58" s="51"/>
+      <c r="B58" s="58"/>
+      <c r="C58" s="54"/>
+      <c r="D58" s="54"/>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B59" s="24">
@@ -4876,33 +4873,33 @@
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B64" s="50">
+      <c r="B64" s="55">
         <v>0.29166666666666702</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D64" s="51"/>
+      <c r="D64" s="54"/>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B65" s="50"/>
+      <c r="B65" s="55"/>
       <c r="C65" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D65" s="51"/>
+      <c r="D65" s="54"/>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B66" s="50"/>
+      <c r="B66" s="55"/>
       <c r="C66" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="D66" s="51"/>
+      <c r="D66" s="54"/>
     </row>
     <row r="67" spans="2:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B67" s="52" t="s">
+      <c r="B67" s="59" t="s">
         <v>99</v>
       </c>
-      <c r="C67" s="51" t="s">
+      <c r="C67" s="54" t="s">
         <v>100</v>
       </c>
       <c r="D67" s="5" t="s">
@@ -4910,8 +4907,8 @@
       </c>
     </row>
     <row r="68" spans="2:4" ht="45" x14ac:dyDescent="0.2">
-      <c r="B68" s="52"/>
-      <c r="C68" s="51"/>
+      <c r="B68" s="59"/>
+      <c r="C68" s="54"/>
       <c r="D68" s="10" t="s">
         <v>102</v>
       </c>
@@ -5008,23 +5005,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="B26:B31"/>
-    <mergeCell ref="D26:D31"/>
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="D46:D47"/>
     <mergeCell ref="B64:B66"/>
     <mergeCell ref="D64:D66"/>
     <mergeCell ref="B67:B68"/>
@@ -5035,6 +5015,23 @@
     <mergeCell ref="B57:B58"/>
     <mergeCell ref="C57:C58"/>
     <mergeCell ref="D57:D58"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="B26:B31"/>
+    <mergeCell ref="D26:D31"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -6457,8 +6454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F445"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6538,19 +6535,19 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="57" t="s">
+      <c r="A6" s="50" t="s">
         <v>325</v>
       </c>
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="50" t="s">
         <v>326</v>
       </c>
-      <c r="C6" s="57" t="s">
+      <c r="C6" s="50" t="s">
         <v>327</v>
       </c>
-      <c r="D6" s="57" t="s">
+      <c r="D6" s="50" t="s">
         <v>328</v>
       </c>
-      <c r="E6" s="57"/>
+      <c r="E6" s="50"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="60" t="s">
@@ -6662,34 +6659,34 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="57" t="s">
+      <c r="A14" s="50" t="s">
         <v>350</v>
       </c>
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="50" t="s">
         <v>351</v>
       </c>
-      <c r="C14" s="57" t="s">
+      <c r="C14" s="50" t="s">
         <v>352</v>
       </c>
-      <c r="D14" s="57" t="s">
+      <c r="D14" s="50" t="s">
         <v>353</v>
       </c>
-      <c r="E14" s="57"/>
+      <c r="E14" s="50"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="57" t="s">
+      <c r="A15" s="50" t="s">
         <v>354</v>
       </c>
-      <c r="B15" s="57" t="s">
+      <c r="B15" s="50" t="s">
         <v>355</v>
       </c>
-      <c r="C15" s="57" t="s">
+      <c r="C15" s="50" t="s">
         <v>352</v>
       </c>
-      <c r="D15" s="57" t="s">
+      <c r="D15" s="50" t="s">
         <v>356</v>
       </c>
-      <c r="E15" s="57"/>
+      <c r="E15" s="50"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -6963,32 +6960,32 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="57" t="s">
+      <c r="A36" s="50" t="s">
         <v>388</v>
       </c>
-      <c r="B36" s="59">
+      <c r="B36" s="52">
         <v>0</v>
       </c>
-      <c r="C36" s="59">
+      <c r="C36" s="52">
         <v>0</v>
       </c>
-      <c r="D36" s="57" t="str">
+      <c r="D36" s="50" t="str">
         <f>A36</f>
         <v>StrokeFAMILY HISTORY</v>
       </c>
-      <c r="E36" s="57"/>
+      <c r="E36" s="50"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="57" t="s">
+      <c r="A37" s="50" t="s">
         <v>389</v>
       </c>
-      <c r="B37" s="59"/>
-      <c r="C37" s="59"/>
-      <c r="D37" s="57" t="str">
+      <c r="B37" s="52"/>
+      <c r="C37" s="52"/>
+      <c r="D37" s="50" t="str">
         <f>A37</f>
         <v>StrokeSpecific FAMILY HISTORY</v>
       </c>
-      <c r="E37" s="57"/>
+      <c r="E37" s="50"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
@@ -7018,36 +7015,36 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="57" t="s">
+      <c r="A40" s="50" t="s">
         <v>393</v>
       </c>
-      <c r="B40" s="59" t="s">
+      <c r="B40" s="52" t="s">
         <v>322</v>
       </c>
-      <c r="C40" s="59" t="s">
+      <c r="C40" s="52" t="s">
         <v>323</v>
       </c>
-      <c r="D40" s="57" t="str">
+      <c r="D40" s="50" t="str">
         <f t="shared" si="1"/>
         <v>STROKE PATIENT MEDICAL HISTORY</v>
       </c>
-      <c r="E40" s="57"/>
+      <c r="E40" s="50"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="57" t="s">
+      <c r="A41" s="50" t="s">
         <v>394</v>
       </c>
-      <c r="B41" s="59" t="s">
+      <c r="B41" s="52" t="s">
         <v>395</v>
       </c>
-      <c r="C41" s="59">
+      <c r="C41" s="52">
         <v>11</v>
       </c>
-      <c r="D41" s="57" t="str">
+      <c r="D41" s="50" t="str">
         <f t="shared" si="1"/>
         <v>STROKE YR PATIENT MEDICAL HISTORY</v>
       </c>
-      <c r="E41" s="57"/>
+      <c r="E41" s="50"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
@@ -7110,80 +7107,80 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="57" t="s">
+      <c r="A46" s="60" t="s">
         <v>401</v>
       </c>
-      <c r="B46" s="59"/>
-      <c r="C46" s="59">
+      <c r="B46" s="62"/>
+      <c r="C46" s="62">
         <v>1994</v>
       </c>
-      <c r="D46" s="57" t="s">
+      <c r="D46" s="60" t="s">
         <v>402</v>
       </c>
-      <c r="E46" s="57" t="s">
+      <c r="E46" s="60" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="57" t="s">
+      <c r="A47" s="50" t="s">
         <v>403</v>
       </c>
-      <c r="B47" s="57"/>
-      <c r="C47" s="57">
+      <c r="B47" s="50"/>
+      <c r="C47" s="50">
         <v>10</v>
       </c>
-      <c r="D47" s="57" t="s">
+      <c r="D47" s="50" t="s">
         <v>404</v>
       </c>
-      <c r="E47" s="58"/>
+      <c r="E47" s="51"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="57" t="s">
+      <c r="A48" s="50" t="s">
         <v>405</v>
       </c>
-      <c r="B48" s="57"/>
-      <c r="C48" s="57">
+      <c r="B48" s="50"/>
+      <c r="C48" s="50">
         <v>3</v>
       </c>
-      <c r="D48" s="57" t="s">
+      <c r="D48" s="50" t="s">
         <v>406</v>
       </c>
-      <c r="E48" s="57"/>
+      <c r="E48" s="50"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="57" t="s">
+      <c r="A49" s="50" t="s">
         <v>407</v>
       </c>
-      <c r="B49" s="57" t="s">
+      <c r="B49" s="50" t="s">
         <v>408</v>
       </c>
-      <c r="C49" s="57" t="s">
+      <c r="C49" s="50" t="s">
         <v>409</v>
       </c>
-      <c r="D49" s="57"/>
-      <c r="E49" s="57"/>
+      <c r="D49" s="50"/>
+      <c r="E49" s="50"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="57" t="s">
+      <c r="A50" s="50" t="s">
         <v>410</v>
       </c>
-      <c r="B50" s="57"/>
-      <c r="C50" s="57" t="s">
+      <c r="B50" s="50"/>
+      <c r="C50" s="50" t="s">
         <v>411</v>
       </c>
-      <c r="D50" s="57"/>
-      <c r="E50" s="57"/>
+      <c r="D50" s="50"/>
+      <c r="E50" s="50"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="57" t="s">
+      <c r="A51" s="50" t="s">
         <v>412</v>
       </c>
-      <c r="B51" s="57"/>
-      <c r="C51" s="57" t="s">
+      <c r="B51" s="50"/>
+      <c r="C51" s="50" t="s">
         <v>413</v>
       </c>
-      <c r="D51" s="57"/>
-      <c r="E51" s="57"/>
+      <c r="D51" s="50"/>
+      <c r="E51" s="50"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">

</xml_diff>